<commit_message>
create cluster label wordalisation
</commit_message>
<xml_diff>
--- a/data/describe/few_shot_cluster.xlsx
+++ b/data/describe/few_shot_cluster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaca253\Documents\datomatisation\datomatisation-dev\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286906C5-9056-4A07-9EC3-81DDA99DAD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDA3D45-B4B5-4AA2-8A46-00ED2261E78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29940" yWindow="1140" windowWidth="38700" windowHeight="15225" xr2:uid="{75A2F0CC-120C-46DD-B882-D3F79246B1DD}"/>
   </bookViews>
@@ -54,13 +54,13 @@
     <t>This cluster reflects individuals who are steady, grounded, and emotionally attuned, often providing a sense of reliability and calm in their interactions. Their main strengths are very high groundedness and relatively high empathy, which allow them to remain composed in challenging situations while understanding and supporting others effectively. On other traits such as modesty, conscientiousness, considerateness, casualness, and slightly lower reservedness, they generally show average tendencies, balancing approachability with thoughtful consideration. Overall, this cluster describes dependable, empathetic individuals who combine strong stability and emotional insight with moderate social and practical traits.</t>
   </si>
   <si>
-    <t>relatively high on outgoing, normal on grounded, normal on modest, conscientious, and considerate, normal on conceptual, normal on meticulous, self-reliant</t>
-  </si>
-  <si>
-    <t>normal on outgoing, normal on pensive, relatively high on outgoing, candid, and cnconventional, slightly high on empathic, normal on casual</t>
-  </si>
-  <si>
-    <t>slightly low on Reserved, very high on grounded, normal on modest, conscientious, and considerate, relatively high on empathic, normal on casual</t>
+    <t>The cluster center can be characterised as: relatively high on outgoing, normal on grounded, normal on modest, conscientious, and considerate, normal on conceptual, normal on meticulous, self-reliant</t>
+  </si>
+  <si>
+    <t>The cluster center can be characterised as: normal on outgoing, normal on pensive, relatively high on outgoing, candid, and conventional, slightly high on empathic, normal on casual</t>
+  </si>
+  <si>
+    <t>The cluster center can be characterised as: slightly low on Reserved, very high on grounded, normal on modest, conscientious, and considerate, relatively high on empathic, normal on casual</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
update wordalisation and visualisation
</commit_message>
<xml_diff>
--- a/data/describe/few_shot_cluster.xlsx
+++ b/data/describe/few_shot_cluster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaca253\Documents\datomatisation\datomatisation-dev\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDA3D45-B4B5-4AA2-8A46-00ED2261E78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CCB1A6-82C8-4F08-8235-A44038701707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="38700" windowHeight="15225" xr2:uid="{75A2F0CC-120C-46DD-B882-D3F79246B1DD}"/>
+    <workbookView xWindow="39900" yWindow="3030" windowWidth="20820" windowHeight="17445" xr2:uid="{75A2F0CC-120C-46DD-B882-D3F79246B1DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,22 +45,28 @@
     <t>Assistant</t>
   </si>
   <si>
-    <t>This cluster represents individuals who are lively, confident, and socially engaging, often bringing energy and enthusiasm to their interactions. Their main strength lies in being highly outgoing, which allows them to connect easily with others and energize social situations. On other traits such as groundedness, modesty, conscientiousness, considerateness, conceptual thinking, meticulousness, and self-reliance, they generally fall within the average range, displaying balanced and steady behavior without extreme tendencies. Overall, this cluster describes sociable, energetic individuals who combine high friendliness and expressiveness with reliably moderate traits across other areas.</t>
-  </si>
-  <si>
-    <t>This cluster includes individuals who are dynamic, open, often approaching situations with a fresh and unconventional perspective. Their key strengths are being relatively outgoing, candid, and willing to break the mold, which helps them connect with others authentically and bring originality to social interactions. Traits like pensive thinking, empathy, and casualness tend to fall in the normal to slightly above-average range, giving them balance and thoughtfulness without extremes. Overall, this cluster represents expressive, inventive individuals who combine boldness and sociability with steady, considerate tendencies.</t>
-  </si>
-  <si>
-    <t>This cluster reflects individuals who are steady, grounded, and emotionally attuned, often providing a sense of reliability and calm in their interactions. Their main strengths are very high groundedness and relatively high empathy, which allow them to remain composed in challenging situations while understanding and supporting others effectively. On other traits such as modesty, conscientiousness, considerateness, casualness, and slightly lower reservedness, they generally show average tendencies, balancing approachability with thoughtful consideration. Overall, this cluster describes dependable, empathetic individuals who combine strong stability and emotional insight with moderate social and practical traits.</t>
-  </si>
-  <si>
-    <t>The cluster center can be characterised as: relatively high on outgoing, normal on grounded, normal on modest, conscientious, and considerate, normal on conceptual, normal on meticulous, self-reliant</t>
-  </si>
-  <si>
     <t>The cluster center can be characterised as: normal on outgoing, normal on pensive, relatively high on outgoing, candid, and conventional, slightly high on empathic, normal on casual</t>
   </si>
   <si>
     <t>The cluster center can be characterised as: slightly low on Reserved, very high on grounded, normal on modest, conscientious, and considerate, relatively high on empathic, normal on casual</t>
+  </si>
+  <si>
+    <t>The cluster center can be characterised as:  slightly low on reserved,  relatively low on worrisome imaginative,  relatively high on outgoing and carefree</t>
+  </si>
+  <si>
+    <t>Entities in this cluster are grounded and empathetic, while being slightly less reserved. They show normal levels of modesty, conscientiousness, and consideration, as well as typical casualness, giving them a stable and thoughtful style.
+Their strengths include being very grounded and relatively empathetic, which helps them stay practical, reliable, and understanding of others.
+Their weaknesses are being slightly reserved.</t>
+  </si>
+  <si>
+    <t>Entities in this cluster are outgoing and carefree, while being slightly less reserved and imaginative, giving them a relaxed and sociable style.
+They are outgoing and carefree, making them comfortable and confident in social settings.
+Their weaknesses are minor being less reserved and imaginative may sometimes lead to less caution, planning, or reflection.</t>
+  </si>
+  <si>
+    <t>Entities in this cluster are generally well-balanced. They show normal levels of outgoing, thoughtful, and casual traits, while being somewhat more outgoing, candid, and conventional, with a bit higher empathy.
+Their strengths include being very outgoing and empathetic, which enables them to communicate clearly, be reliable, and understand others well.
+Their weaknesses are minor since most traits are normal, but being slightly too conventional might sometimes limit flexibility or creativity.</t>
   </si>
 </sst>
 </file>
@@ -425,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A39C770-6B8C-4FC7-97FD-94B205744AFD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,28 +449,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="210" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="140" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="182" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="232" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>